<commit_message>
Add thickness to tables
</commit_message>
<xml_diff>
--- a/analysis/tables/table_topsites.xlsx
+++ b/analysis/tables/table_topsites.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="filtered_sites_with_ranking" sheetId="1" r:id="rId1"/>
+    <sheet name="filtered_sites_cti_ranking" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,32 +360,37 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>sitename</t>
+          <t>Site</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>igbp_land_use</t>
+          <t>LCT</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>cti</t>
+          <t>CTI</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>res_cond</t>
+          <t>Res</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>aridity_class</t>
+          <t>Aridity</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cti_class</t>
+          <t>CTI_Class</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Thk</t>
         </is>
       </c>
     </row>
@@ -416,6 +421,9 @@
           <t>Very High</t>
         </is>
       </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -444,6 +452,9 @@
           <t>Very High</t>
         </is>
       </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -472,6 +483,9 @@
           <t>High</t>
         </is>
       </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -500,6 +514,9 @@
           <t>High</t>
         </is>
       </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -528,6 +545,9 @@
           <t>High</t>
         </is>
       </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -556,6 +576,9 @@
           <t>High</t>
         </is>
       </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -584,6 +607,9 @@
           <t>Medium</t>
         </is>
       </c>
+      <c r="G8">
+        <v>39</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -611,6 +637,9 @@
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="G9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>